<commit_message>
Updated Sprint Backlog and Sprint Review
</commit_message>
<xml_diff>
--- a/Deliverable_2_Documents/FiveGuys_Deliverable_2_Sprint_Backlog.xlsx
+++ b/Deliverable_2_Documents/FiveGuys_Deliverable_2_Sprint_Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xinophilius\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spencer\Desktop\COS 420\Git\FiveGuys_420Project\Deliverable_2_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6944C764-AA31-4C5C-8F6C-44C56359DE99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC3BE27-9B5A-4E49-B901-247AE04B2BB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Sprint Goal &amp; Number</t>
   </si>
@@ -55,19 +55,25 @@
     <t>Overall: Enable 2 player local mode</t>
   </si>
   <si>
-    <t>Represent 4x4 board and pieces via text to console</t>
-  </si>
-  <si>
-    <t>Enable placing of pieces on 4x4 board via text command</t>
-  </si>
-  <si>
-    <t>Recognize victory conditions of 4 in a row same quality pieces</t>
-  </si>
-  <si>
     <t>7 total</t>
   </si>
   <si>
     <t>User Story ID</t>
+  </si>
+  <si>
+    <t>Create sprites for pieces and board</t>
+  </si>
+  <si>
+    <t>Represent 4x4 board and pieces via Unity</t>
+  </si>
+  <si>
+    <t>Enable placing of pieces on 4x4 board via drag and drop</t>
+  </si>
+  <si>
+    <t>Austin/Spencer</t>
+  </si>
+  <si>
+    <t>Initial protoype and complete and functioning. Game mechanics are coming next.</t>
   </si>
 </sst>
 </file>
@@ -350,8 +356,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -372,7 +378,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -414,7 +420,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -425,31 +431,40 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="2">
-        <v>3</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
@@ -458,14 +473,18 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>

</xml_diff>